<commit_message>
feat: project development plan
</commit_message>
<xml_diff>
--- a/Smt 3/Project Management/Week 9 - Midterm/Group 4 - Room Tenant System.xlsx
+++ b/Smt 3/Project Management/Week 9 - Midterm/Group 4 - Room Tenant System.xlsx
@@ -1,38 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27203"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FD68A81-B985-4CD5-BD36-3A86EC6AE97C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Smt 3\Project Management\Week 9 - Midterm\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60EEC66-7FD7-46D1-9064-96066C20E825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="1" r:id="rId1"/>
     <sheet name="Cost Estimate" sheetId="2" r:id="rId2"/>
+    <sheet name="Init" sheetId="3" r:id="rId3"/>
+    <sheet name="Plan" sheetId="4" r:id="rId4"/>
+    <sheet name="Exec" sheetId="5" r:id="rId5"/>
+    <sheet name="Ctrl" sheetId="6" r:id="rId6"/>
+    <sheet name="Clos" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="67">
   <si>
     <t>Room Tenant System</t>
   </si>
@@ -243,7 +242,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-13809]dd\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,7 +406,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -731,11 +730,307 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -909,33 +1204,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -954,12 +1222,105 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1279,14 +1640,14 @@
   </sheetPr>
   <dimension ref="B1:CD50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="6" ySplit="9" topLeftCell="G10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.5703125" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="4.5703125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="2" max="2" width="45.7109375" customWidth="1"/>
@@ -1294,32 +1655,32 @@
     <col min="4" max="5" width="13.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:82" ht="30" customHeight="1">
+    <row r="1" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
     </row>
-    <row r="2" spans="2:82" ht="30" customHeight="1">
+    <row r="2" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="59"/>
       <c r="C2" s="59"/>
       <c r="D2" s="59"/>
       <c r="E2" s="59"/>
       <c r="F2" s="59"/>
     </row>
-    <row r="3" spans="2:82" ht="30" customHeight="1">
-      <c r="B3" s="106" t="s">
+    <row r="3" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
       <c r="F3" s="60"/>
     </row>
-    <row r="4" spans="2:82" ht="30" customHeight="1">
-      <c r="B4" s="106"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
+    <row r="4" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="114"/>
+      <c r="C4" s="114"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
       <c r="F4" s="60"/>
       <c r="G4" s="59"/>
       <c r="H4" s="59"/>
@@ -1400,11 +1761,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:82" ht="30" customHeight="1">
-      <c r="B5" s="106"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
+    <row r="5" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="114"/>
+      <c r="C5" s="114"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
       <c r="F5" s="60"/>
       <c r="G5" s="59"/>
       <c r="H5" s="59"/>
@@ -1485,221 +1846,221 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:82" ht="30" customHeight="1">
-      <c r="B6" s="103" t="s">
+    <row r="6" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="104" t="s">
+      <c r="C6" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
       <c r="F6" s="61"/>
-      <c r="G6" s="99">
+      <c r="G6" s="105">
         <v>45222</v>
       </c>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="99">
+      <c r="H6" s="106"/>
+      <c r="I6" s="106"/>
+      <c r="J6" s="106"/>
+      <c r="K6" s="106"/>
+      <c r="L6" s="105">
         <v>45229</v>
       </c>
-      <c r="M6" s="100"/>
-      <c r="N6" s="100"/>
-      <c r="O6" s="100"/>
-      <c r="P6" s="100"/>
-      <c r="Q6" s="99">
+      <c r="M6" s="106"/>
+      <c r="N6" s="106"/>
+      <c r="O6" s="106"/>
+      <c r="P6" s="106"/>
+      <c r="Q6" s="105">
         <v>45236</v>
       </c>
-      <c r="R6" s="100"/>
-      <c r="S6" s="100"/>
-      <c r="T6" s="100"/>
-      <c r="U6" s="100"/>
-      <c r="V6" s="99">
+      <c r="R6" s="106"/>
+      <c r="S6" s="106"/>
+      <c r="T6" s="106"/>
+      <c r="U6" s="106"/>
+      <c r="V6" s="105">
         <v>45243</v>
       </c>
-      <c r="W6" s="100"/>
-      <c r="X6" s="100"/>
-      <c r="Y6" s="100"/>
-      <c r="Z6" s="100"/>
-      <c r="AA6" s="99">
+      <c r="W6" s="106"/>
+      <c r="X6" s="106"/>
+      <c r="Y6" s="106"/>
+      <c r="Z6" s="106"/>
+      <c r="AA6" s="105">
         <v>45250</v>
       </c>
-      <c r="AB6" s="100"/>
-      <c r="AC6" s="100"/>
-      <c r="AD6" s="100"/>
-      <c r="AE6" s="100"/>
-      <c r="AF6" s="99">
+      <c r="AB6" s="106"/>
+      <c r="AC6" s="106"/>
+      <c r="AD6" s="106"/>
+      <c r="AE6" s="106"/>
+      <c r="AF6" s="105">
         <v>45257</v>
       </c>
-      <c r="AG6" s="100"/>
-      <c r="AH6" s="100"/>
-      <c r="AI6" s="100"/>
-      <c r="AJ6" s="100"/>
-      <c r="AK6" s="99">
+      <c r="AG6" s="106"/>
+      <c r="AH6" s="106"/>
+      <c r="AI6" s="106"/>
+      <c r="AJ6" s="106"/>
+      <c r="AK6" s="105">
         <v>45264</v>
       </c>
-      <c r="AL6" s="100"/>
-      <c r="AM6" s="100"/>
-      <c r="AN6" s="100"/>
-      <c r="AO6" s="100"/>
-      <c r="AP6" s="99">
+      <c r="AL6" s="106"/>
+      <c r="AM6" s="106"/>
+      <c r="AN6" s="106"/>
+      <c r="AO6" s="106"/>
+      <c r="AP6" s="105">
         <v>45271</v>
       </c>
-      <c r="AQ6" s="100"/>
-      <c r="AR6" s="100"/>
-      <c r="AS6" s="100"/>
-      <c r="AT6" s="100"/>
-      <c r="AU6" s="99">
+      <c r="AQ6" s="106"/>
+      <c r="AR6" s="106"/>
+      <c r="AS6" s="106"/>
+      <c r="AT6" s="106"/>
+      <c r="AU6" s="105">
         <v>45278</v>
       </c>
-      <c r="AV6" s="100"/>
-      <c r="AW6" s="100"/>
-      <c r="AX6" s="100"/>
-      <c r="AY6" s="100"/>
-      <c r="AZ6" s="99">
+      <c r="AV6" s="106"/>
+      <c r="AW6" s="106"/>
+      <c r="AX6" s="106"/>
+      <c r="AY6" s="106"/>
+      <c r="AZ6" s="105">
         <v>45285</v>
       </c>
-      <c r="BA6" s="100"/>
-      <c r="BB6" s="100"/>
-      <c r="BC6" s="100"/>
-      <c r="BD6" s="100"/>
-      <c r="BE6" s="99">
+      <c r="BA6" s="106"/>
+      <c r="BB6" s="106"/>
+      <c r="BC6" s="106"/>
+      <c r="BD6" s="106"/>
+      <c r="BE6" s="105">
         <v>45292</v>
       </c>
-      <c r="BF6" s="100"/>
-      <c r="BG6" s="100"/>
-      <c r="BH6" s="100"/>
-      <c r="BI6" s="100"/>
-      <c r="BJ6" s="108">
+      <c r="BF6" s="106"/>
+      <c r="BG6" s="106"/>
+      <c r="BH6" s="106"/>
+      <c r="BI6" s="106"/>
+      <c r="BJ6" s="99">
         <v>45299</v>
       </c>
-      <c r="BK6" s="109"/>
-      <c r="BL6" s="109"/>
-      <c r="BM6" s="109"/>
-      <c r="BN6" s="110"/>
-      <c r="BO6" s="99">
+      <c r="BK6" s="100"/>
+      <c r="BL6" s="100"/>
+      <c r="BM6" s="100"/>
+      <c r="BN6" s="101"/>
+      <c r="BO6" s="105">
         <v>45306</v>
       </c>
-      <c r="BP6" s="100"/>
-      <c r="BQ6" s="100"/>
-      <c r="BR6" s="100"/>
-      <c r="BS6" s="100"/>
-      <c r="BT6" s="108">
+      <c r="BP6" s="106"/>
+      <c r="BQ6" s="106"/>
+      <c r="BR6" s="106"/>
+      <c r="BS6" s="106"/>
+      <c r="BT6" s="99">
         <v>45313</v>
       </c>
-      <c r="BU6" s="109"/>
-      <c r="BV6" s="109"/>
-      <c r="BW6" s="109"/>
-      <c r="BX6" s="110"/>
-      <c r="BY6" s="108">
+      <c r="BU6" s="100"/>
+      <c r="BV6" s="100"/>
+      <c r="BW6" s="100"/>
+      <c r="BX6" s="101"/>
+      <c r="BY6" s="99">
         <v>45320</v>
       </c>
-      <c r="BZ6" s="109"/>
-      <c r="CA6" s="109"/>
-      <c r="CB6" s="109"/>
-      <c r="CC6" s="114"/>
+      <c r="BZ6" s="100"/>
+      <c r="CA6" s="100"/>
+      <c r="CB6" s="100"/>
+      <c r="CC6" s="109"/>
       <c r="CD6" s="59" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:82" ht="30" customHeight="1">
-      <c r="B7" s="103"/>
-      <c r="C7" s="105" t="s">
+    <row r="7" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="111"/>
+      <c r="C7" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="105"/>
-      <c r="E7" s="105"/>
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
       <c r="F7" s="62"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="102"/>
-      <c r="I7" s="102"/>
-      <c r="J7" s="102"/>
-      <c r="K7" s="102"/>
-      <c r="L7" s="101"/>
-      <c r="M7" s="102"/>
-      <c r="N7" s="102"/>
-      <c r="O7" s="102"/>
-      <c r="P7" s="102"/>
-      <c r="Q7" s="101"/>
-      <c r="R7" s="102"/>
-      <c r="S7" s="102"/>
-      <c r="T7" s="102"/>
-      <c r="U7" s="102"/>
-      <c r="V7" s="101"/>
-      <c r="W7" s="102"/>
-      <c r="X7" s="102"/>
-      <c r="Y7" s="102"/>
-      <c r="Z7" s="102"/>
-      <c r="AA7" s="101"/>
-      <c r="AB7" s="102"/>
-      <c r="AC7" s="102"/>
-      <c r="AD7" s="102"/>
-      <c r="AE7" s="102"/>
-      <c r="AF7" s="101"/>
-      <c r="AG7" s="102"/>
-      <c r="AH7" s="102"/>
-      <c r="AI7" s="102"/>
-      <c r="AJ7" s="102"/>
-      <c r="AK7" s="101"/>
-      <c r="AL7" s="102"/>
-      <c r="AM7" s="102"/>
-      <c r="AN7" s="102"/>
-      <c r="AO7" s="102"/>
-      <c r="AP7" s="101"/>
-      <c r="AQ7" s="102"/>
-      <c r="AR7" s="102"/>
-      <c r="AS7" s="102"/>
-      <c r="AT7" s="102"/>
-      <c r="AU7" s="101"/>
-      <c r="AV7" s="102"/>
-      <c r="AW7" s="102"/>
-      <c r="AX7" s="102"/>
-      <c r="AY7" s="102"/>
-      <c r="AZ7" s="101"/>
-      <c r="BA7" s="102"/>
-      <c r="BB7" s="102"/>
-      <c r="BC7" s="102"/>
-      <c r="BD7" s="102"/>
-      <c r="BE7" s="101"/>
-      <c r="BF7" s="102"/>
-      <c r="BG7" s="102"/>
-      <c r="BH7" s="102"/>
-      <c r="BI7" s="102"/>
-      <c r="BJ7" s="111"/>
-      <c r="BK7" s="112"/>
-      <c r="BL7" s="112"/>
-      <c r="BM7" s="112"/>
-      <c r="BN7" s="113"/>
-      <c r="BO7" s="101"/>
-      <c r="BP7" s="102"/>
-      <c r="BQ7" s="102"/>
-      <c r="BR7" s="102"/>
-      <c r="BS7" s="102"/>
-      <c r="BT7" s="111"/>
-      <c r="BU7" s="112"/>
-      <c r="BV7" s="112"/>
-      <c r="BW7" s="112"/>
-      <c r="BX7" s="113"/>
-      <c r="BY7" s="111"/>
-      <c r="BZ7" s="112"/>
-      <c r="CA7" s="112"/>
-      <c r="CB7" s="112"/>
-      <c r="CC7" s="115"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="108"/>
+      <c r="I7" s="108"/>
+      <c r="J7" s="108"/>
+      <c r="K7" s="108"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="108"/>
+      <c r="N7" s="108"/>
+      <c r="O7" s="108"/>
+      <c r="P7" s="108"/>
+      <c r="Q7" s="107"/>
+      <c r="R7" s="108"/>
+      <c r="S7" s="108"/>
+      <c r="T7" s="108"/>
+      <c r="U7" s="108"/>
+      <c r="V7" s="107"/>
+      <c r="W7" s="108"/>
+      <c r="X7" s="108"/>
+      <c r="Y7" s="108"/>
+      <c r="Z7" s="108"/>
+      <c r="AA7" s="107"/>
+      <c r="AB7" s="108"/>
+      <c r="AC7" s="108"/>
+      <c r="AD7" s="108"/>
+      <c r="AE7" s="108"/>
+      <c r="AF7" s="107"/>
+      <c r="AG7" s="108"/>
+      <c r="AH7" s="108"/>
+      <c r="AI7" s="108"/>
+      <c r="AJ7" s="108"/>
+      <c r="AK7" s="107"/>
+      <c r="AL7" s="108"/>
+      <c r="AM7" s="108"/>
+      <c r="AN7" s="108"/>
+      <c r="AO7" s="108"/>
+      <c r="AP7" s="107"/>
+      <c r="AQ7" s="108"/>
+      <c r="AR7" s="108"/>
+      <c r="AS7" s="108"/>
+      <c r="AT7" s="108"/>
+      <c r="AU7" s="107"/>
+      <c r="AV7" s="108"/>
+      <c r="AW7" s="108"/>
+      <c r="AX7" s="108"/>
+      <c r="AY7" s="108"/>
+      <c r="AZ7" s="107"/>
+      <c r="BA7" s="108"/>
+      <c r="BB7" s="108"/>
+      <c r="BC7" s="108"/>
+      <c r="BD7" s="108"/>
+      <c r="BE7" s="107"/>
+      <c r="BF7" s="108"/>
+      <c r="BG7" s="108"/>
+      <c r="BH7" s="108"/>
+      <c r="BI7" s="108"/>
+      <c r="BJ7" s="102"/>
+      <c r="BK7" s="103"/>
+      <c r="BL7" s="103"/>
+      <c r="BM7" s="103"/>
+      <c r="BN7" s="104"/>
+      <c r="BO7" s="107"/>
+      <c r="BP7" s="108"/>
+      <c r="BQ7" s="108"/>
+      <c r="BR7" s="108"/>
+      <c r="BS7" s="108"/>
+      <c r="BT7" s="102"/>
+      <c r="BU7" s="103"/>
+      <c r="BV7" s="103"/>
+      <c r="BW7" s="103"/>
+      <c r="BX7" s="104"/>
+      <c r="BY7" s="102"/>
+      <c r="BZ7" s="103"/>
+      <c r="CA7" s="103"/>
+      <c r="CB7" s="103"/>
+      <c r="CC7" s="110"/>
       <c r="CD7" s="59" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:82" ht="30" customHeight="1">
-      <c r="B8" s="107" t="s">
+    <row r="8" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="107"/>
-      <c r="D8" s="107" t="s">
+      <c r="C8" s="115"/>
+      <c r="D8" s="115" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="107" t="s">
+      <c r="E8" s="115" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="61"/>
@@ -1932,11 +2293,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:82" ht="30" customHeight="1">
-      <c r="B9" s="107"/>
-      <c r="C9" s="107"/>
-      <c r="D9" s="107"/>
-      <c r="E9" s="107"/>
+    <row r="9" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="115"/>
+      <c r="C9" s="115"/>
+      <c r="D9" s="115"/>
+      <c r="E9" s="115"/>
       <c r="F9" s="61"/>
       <c r="G9" s="86" t="s">
         <v>8</v>
@@ -2167,7 +2528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:82" ht="30" customHeight="1">
+    <row r="10" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="18" t="s">
         <v>12</v>
       </c>
@@ -2254,7 +2615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:82" ht="30" customHeight="1">
+    <row r="11" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
         <v>13</v>
       </c>
@@ -2345,7 +2706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:82" ht="30" customHeight="1">
+    <row r="12" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
         <v>14</v>
       </c>
@@ -2436,7 +2797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:82" ht="30" customHeight="1">
+    <row r="13" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
         <v>15</v>
       </c>
@@ -2527,7 +2888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:82" ht="30" customHeight="1">
+    <row r="14" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
         <v>16</v>
       </c>
@@ -2618,7 +2979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:82" ht="30" customHeight="1">
+    <row r="15" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="23" t="s">
         <v>17</v>
       </c>
@@ -2709,7 +3070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:82" ht="30" customHeight="1">
+    <row r="16" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="23" t="s">
         <v>18</v>
       </c>
@@ -2800,7 +3161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:82" ht="30" customHeight="1">
+    <row r="17" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
         <v>19</v>
       </c>
@@ -2891,7 +3252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:82" ht="30" customHeight="1">
+    <row r="18" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="23" t="s">
         <v>20</v>
       </c>
@@ -2982,7 +3343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:82" ht="30" customHeight="1">
+    <row r="19" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="19" t="s">
         <v>21</v>
       </c>
@@ -3069,7 +3430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:82" ht="30" customHeight="1">
+    <row r="20" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="24" t="s">
         <v>22</v>
       </c>
@@ -3160,7 +3521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:82" ht="30" customHeight="1">
+    <row r="21" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="24" t="s">
         <v>23</v>
       </c>
@@ -3251,7 +3612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:82" ht="30" customHeight="1">
+    <row r="22" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="24" t="s">
         <v>24</v>
       </c>
@@ -3342,7 +3703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:82" ht="30" customHeight="1">
+    <row r="23" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="24" t="s">
         <v>25</v>
       </c>
@@ -3433,7 +3794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:82" ht="30" customHeight="1">
+    <row r="24" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="24" t="s">
         <v>26</v>
       </c>
@@ -3524,7 +3885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:82" ht="30" customHeight="1">
+    <row r="25" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="24" t="s">
         <v>27</v>
       </c>
@@ -3615,7 +3976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:82" ht="30" customHeight="1">
+    <row r="26" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="24" t="s">
         <v>28</v>
       </c>
@@ -3706,7 +4067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:82" ht="30" customHeight="1">
+    <row r="27" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="20" t="s">
         <v>29</v>
       </c>
@@ -3793,7 +4154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:82" ht="30" customHeight="1">
+    <row r="28" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="25" t="s">
         <v>30</v>
       </c>
@@ -3884,7 +4245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:82" ht="30" customHeight="1">
+    <row r="29" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="25" t="s">
         <v>31</v>
       </c>
@@ -3975,7 +4336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:82" ht="30" customHeight="1">
+    <row r="30" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="25" t="s">
         <v>32</v>
       </c>
@@ -4066,7 +4427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:82" ht="30" customHeight="1">
+    <row r="31" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="25" t="s">
         <v>33</v>
       </c>
@@ -4157,7 +4518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:82" ht="30" customHeight="1">
+    <row r="32" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="25" t="s">
         <v>34</v>
       </c>
@@ -4248,7 +4609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:82" ht="30" customHeight="1">
+    <row r="33" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="25" t="s">
         <v>35</v>
       </c>
@@ -4339,7 +4700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:82" ht="30" customHeight="1">
+    <row r="34" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="25" t="s">
         <v>36</v>
       </c>
@@ -4430,7 +4791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:82" ht="30" customHeight="1">
+    <row r="35" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="25" t="s">
         <v>37</v>
       </c>
@@ -4521,7 +4882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:82" ht="30" customHeight="1">
+    <row r="36" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="25" t="s">
         <v>38</v>
       </c>
@@ -4612,7 +4973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:82" ht="30" customHeight="1">
+    <row r="37" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="21" t="s">
         <v>39</v>
       </c>
@@ -4699,7 +5060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:82" ht="30" customHeight="1">
+    <row r="38" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="26" t="s">
         <v>40</v>
       </c>
@@ -4790,7 +5151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:82" ht="30" customHeight="1">
+    <row r="39" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="26" t="s">
         <v>41</v>
       </c>
@@ -4881,7 +5242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:82" ht="30" customHeight="1">
+    <row r="40" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="26" t="s">
         <v>42</v>
       </c>
@@ -4972,7 +5333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:82" ht="30" customHeight="1">
+    <row r="41" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="26" t="s">
         <v>43</v>
       </c>
@@ -5063,7 +5424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:82" ht="30" customHeight="1">
+    <row r="42" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="26" t="s">
         <v>44</v>
       </c>
@@ -5154,7 +5515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:82" ht="30" customHeight="1">
+    <row r="43" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B43" s="22" t="s">
         <v>45</v>
       </c>
@@ -5241,7 +5602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:82" ht="30" customHeight="1">
+    <row r="44" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="27" t="s">
         <v>46</v>
       </c>
@@ -5332,7 +5693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:82" ht="30" customHeight="1">
+    <row r="45" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="27" t="s">
         <v>47</v>
       </c>
@@ -5423,7 +5784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:82" ht="30" customHeight="1">
+    <row r="46" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="27" t="s">
         <v>48</v>
       </c>
@@ -5514,7 +5875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:82" ht="30" customHeight="1">
+    <row r="47" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="27" t="s">
         <v>49</v>
       </c>
@@ -5605,7 +5966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:82" ht="30" customHeight="1">
+    <row r="48" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="27" t="s">
         <v>50</v>
       </c>
@@ -5696,7 +6057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:82" ht="30" customHeight="1">
+    <row r="49" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="27" t="s">
         <v>51</v>
       </c>
@@ -5787,7 +6148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:82" ht="30" customHeight="1">
+    <row r="50" spans="2:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="27" t="s">
         <v>52</v>
       </c>
@@ -6030,6 +6391,19 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="G6:K7"/>
+    <mergeCell ref="L6:P7"/>
+    <mergeCell ref="AU6:AY7"/>
+    <mergeCell ref="AZ6:BD7"/>
+    <mergeCell ref="BE6:BI7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="B3:E5"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
     <mergeCell ref="BJ6:BN7"/>
     <mergeCell ref="BO6:BS7"/>
     <mergeCell ref="BT6:BX7"/>
@@ -6040,19 +6414,6 @@
     <mergeCell ref="AF6:AJ7"/>
     <mergeCell ref="AK6:AO7"/>
     <mergeCell ref="AP6:AT7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="B3:E5"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="G6:K7"/>
-    <mergeCell ref="L6:P7"/>
-    <mergeCell ref="AU6:AY7"/>
-    <mergeCell ref="AZ6:BD7"/>
-    <mergeCell ref="BE6:BI7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" fitToHeight="0" orientation="landscape"/>
@@ -6067,14 +6428,14 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="2" max="2" width="45.7109375" customWidth="1"/>
     <col min="3" max="5" width="18.28515625" style="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="30" customHeight="1">
+    <row r="2" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="57" t="s">
         <v>53</v>
       </c>
@@ -6088,7 +6449,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="30" customHeight="1">
+    <row r="3" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="45" t="s">
         <v>57</v>
       </c>
@@ -6099,7 +6460,7 @@
         <v>107675000</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="30" customHeight="1">
+    <row r="4" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="47" t="s">
         <v>58</v>
       </c>
@@ -6114,7 +6475,7 @@
         <v>23725000</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="30" customHeight="1">
+    <row r="5" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="47" t="s">
         <v>59</v>
       </c>
@@ -6130,7 +6491,7 @@
         <v>43800000</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="30" customHeight="1">
+    <row r="6" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="47" t="s">
         <v>60</v>
       </c>
@@ -6146,7 +6507,7 @@
         <v>18250000</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="30" customHeight="1">
+    <row r="7" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="47" t="s">
         <v>61</v>
       </c>
@@ -6162,7 +6523,7 @@
         <v>21900000</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="30" customHeight="1">
+    <row r="8" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="49" t="s">
         <v>62</v>
       </c>
@@ -6173,7 +6534,7 @@
         <v>8120000</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="30" customHeight="1">
+    <row r="9" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="51" t="s">
         <v>63</v>
       </c>
@@ -6188,7 +6549,7 @@
         <v>8000000</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="30" customHeight="1">
+    <row r="10" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="51" t="s">
         <v>64</v>
       </c>
@@ -6203,7 +6564,7 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="30" customHeight="1">
+    <row r="11" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="53" t="s">
         <v>65</v>
       </c>
@@ -6214,7 +6575,7 @@
         <v>23160000</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="30" customHeight="1">
+    <row r="12" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="55" t="s">
         <v>66</v>
       </c>
@@ -6228,4 +6589,3369 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD80E4C2-526D-4E96-A69B-CCFE96AD55BE}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:AA18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:AA18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.5703125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1"/>
+    </row>
+    <row r="2" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="136"/>
+      <c r="M2" s="136"/>
+      <c r="N2" s="136"/>
+      <c r="O2" s="136"/>
+      <c r="P2" s="136"/>
+      <c r="Q2" s="136"/>
+      <c r="R2" s="136"/>
+      <c r="S2" s="136"/>
+      <c r="T2" s="136"/>
+      <c r="U2" s="136"/>
+      <c r="V2" s="136"/>
+      <c r="W2" s="136"/>
+      <c r="X2" s="136"/>
+      <c r="Y2" s="136"/>
+      <c r="Z2" s="136"/>
+      <c r="AA2" s="136"/>
+    </row>
+    <row r="3" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="114" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="136"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="136"/>
+      <c r="J3" s="136"/>
+      <c r="K3" s="136"/>
+      <c r="L3" s="136"/>
+      <c r="M3" s="136"/>
+      <c r="N3" s="136"/>
+      <c r="O3" s="136"/>
+      <c r="P3" s="136"/>
+      <c r="Q3" s="136"/>
+      <c r="R3" s="136"/>
+      <c r="S3" s="136"/>
+      <c r="T3" s="136"/>
+      <c r="U3" s="136"/>
+      <c r="V3" s="136"/>
+      <c r="W3" s="136"/>
+      <c r="X3" s="136"/>
+      <c r="Y3" s="136"/>
+      <c r="Z3" s="136"/>
+      <c r="AA3" s="136"/>
+    </row>
+    <row r="4" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="114"/>
+      <c r="C4" s="114"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59"/>
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="59"/>
+      <c r="W4" s="59"/>
+      <c r="X4" s="59"/>
+      <c r="Y4" s="59"/>
+      <c r="Z4" s="59"/>
+      <c r="AA4" s="59"/>
+    </row>
+    <row r="5" spans="2:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="114"/>
+      <c r="C5" s="114"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="59"/>
+      <c r="R5" s="59"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="59"/>
+      <c r="V5" s="59"/>
+      <c r="W5" s="59"/>
+      <c r="X5" s="59"/>
+      <c r="Y5" s="59"/>
+      <c r="Z5" s="59"/>
+      <c r="AA5" s="59"/>
+    </row>
+    <row r="6" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="111" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="112" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="116">
+        <v>45222</v>
+      </c>
+      <c r="H6" s="117"/>
+      <c r="I6" s="117"/>
+      <c r="J6" s="117"/>
+      <c r="K6" s="117"/>
+      <c r="L6" s="118">
+        <v>45229</v>
+      </c>
+      <c r="M6" s="117"/>
+      <c r="N6" s="117"/>
+      <c r="O6" s="117"/>
+      <c r="P6" s="117"/>
+      <c r="Q6" s="118">
+        <v>45236</v>
+      </c>
+      <c r="R6" s="117"/>
+      <c r="S6" s="117"/>
+      <c r="T6" s="117"/>
+      <c r="U6" s="117"/>
+      <c r="V6" s="118">
+        <v>45243</v>
+      </c>
+      <c r="W6" s="117"/>
+      <c r="X6" s="117"/>
+      <c r="Y6" s="117"/>
+      <c r="Z6" s="119"/>
+      <c r="AA6" s="59"/>
+    </row>
+    <row r="7" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="111"/>
+      <c r="C7" s="113" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="120"/>
+      <c r="H7" s="108"/>
+      <c r="I7" s="108"/>
+      <c r="J7" s="108"/>
+      <c r="K7" s="108"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="108"/>
+      <c r="N7" s="108"/>
+      <c r="O7" s="108"/>
+      <c r="P7" s="108"/>
+      <c r="Q7" s="107"/>
+      <c r="R7" s="108"/>
+      <c r="S7" s="108"/>
+      <c r="T7" s="108"/>
+      <c r="U7" s="108"/>
+      <c r="V7" s="107"/>
+      <c r="W7" s="108"/>
+      <c r="X7" s="108"/>
+      <c r="Y7" s="108"/>
+      <c r="Z7" s="121"/>
+      <c r="AA7" s="59"/>
+    </row>
+    <row r="8" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="115" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="115"/>
+      <c r="D8" s="115" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="115" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="61"/>
+      <c r="G8" s="122">
+        <v>23</v>
+      </c>
+      <c r="H8" s="29">
+        <v>24</v>
+      </c>
+      <c r="I8" s="29">
+        <v>25</v>
+      </c>
+      <c r="J8" s="29">
+        <v>26</v>
+      </c>
+      <c r="K8" s="39">
+        <v>27</v>
+      </c>
+      <c r="L8" s="63">
+        <v>30</v>
+      </c>
+      <c r="M8" s="29">
+        <v>31</v>
+      </c>
+      <c r="N8" s="29">
+        <v>1</v>
+      </c>
+      <c r="O8" s="29">
+        <v>2</v>
+      </c>
+      <c r="P8" s="39">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="63">
+        <v>6</v>
+      </c>
+      <c r="R8" s="29">
+        <v>7</v>
+      </c>
+      <c r="S8" s="29">
+        <v>8</v>
+      </c>
+      <c r="T8" s="29">
+        <v>9</v>
+      </c>
+      <c r="U8" s="39">
+        <v>10</v>
+      </c>
+      <c r="V8" s="63">
+        <v>13</v>
+      </c>
+      <c r="W8" s="29">
+        <v>14</v>
+      </c>
+      <c r="X8" s="29">
+        <v>15</v>
+      </c>
+      <c r="Y8" s="29">
+        <v>16</v>
+      </c>
+      <c r="Z8" s="123">
+        <v>17</v>
+      </c>
+      <c r="AA8" s="59"/>
+    </row>
+    <row r="9" spans="2:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="115"/>
+      <c r="C9" s="115"/>
+      <c r="D9" s="115"/>
+      <c r="E9" s="115"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="124" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="P9" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="R9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="S9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="T9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="U9" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="V9" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="W9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="X9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z9" s="125" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA9" s="59"/>
+    </row>
+    <row r="10" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="126"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="84"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="83"/>
+      <c r="N10" s="83"/>
+      <c r="O10" s="83"/>
+      <c r="P10" s="84"/>
+      <c r="Q10" s="82"/>
+      <c r="R10" s="83"/>
+      <c r="S10" s="83"/>
+      <c r="T10" s="83"/>
+      <c r="U10" s="84"/>
+      <c r="V10" s="82"/>
+      <c r="W10" s="83"/>
+      <c r="X10" s="83"/>
+      <c r="Y10" s="83"/>
+      <c r="Z10" s="127"/>
+      <c r="AA10" s="59"/>
+    </row>
+    <row r="11" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="8">
+        <v>45224</v>
+      </c>
+      <c r="E11" s="8">
+        <v>45225</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="128"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="65"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="40"/>
+      <c r="V11" s="65"/>
+      <c r="W11" s="30"/>
+      <c r="X11" s="30"/>
+      <c r="Y11" s="30"/>
+      <c r="Z11" s="129"/>
+      <c r="AA11" s="59"/>
+    </row>
+    <row r="12" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="8">
+        <v>45226</v>
+      </c>
+      <c r="E12" s="8">
+        <v>45227</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="128"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="69"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="65"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="30"/>
+      <c r="U12" s="40"/>
+      <c r="V12" s="65"/>
+      <c r="W12" s="30"/>
+      <c r="X12" s="30"/>
+      <c r="Y12" s="30"/>
+      <c r="Z12" s="129"/>
+      <c r="AA12" s="59"/>
+    </row>
+    <row r="13" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="8">
+        <v>45228</v>
+      </c>
+      <c r="E13" s="8">
+        <v>45229</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="128"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="65"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="65"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30"/>
+      <c r="U13" s="40"/>
+      <c r="V13" s="65"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="30"/>
+      <c r="Y13" s="30"/>
+      <c r="Z13" s="129"/>
+      <c r="AA13" s="59"/>
+    </row>
+    <row r="14" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="8">
+        <v>45230</v>
+      </c>
+      <c r="E14" s="8">
+        <v>45230</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="128"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="65"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
+      <c r="U14" s="40"/>
+      <c r="V14" s="65"/>
+      <c r="W14" s="30"/>
+      <c r="X14" s="30"/>
+      <c r="Y14" s="30"/>
+      <c r="Z14" s="129"/>
+      <c r="AA14" s="59"/>
+    </row>
+    <row r="15" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="8">
+        <v>45231</v>
+      </c>
+      <c r="E15" s="8">
+        <v>45232</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="128"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="70"/>
+      <c r="Q15" s="69"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="30"/>
+      <c r="U15" s="40"/>
+      <c r="V15" s="65"/>
+      <c r="W15" s="30"/>
+      <c r="X15" s="30"/>
+      <c r="Y15" s="30"/>
+      <c r="Z15" s="129"/>
+      <c r="AA15" s="59"/>
+    </row>
+    <row r="16" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="8">
+        <v>45233</v>
+      </c>
+      <c r="E16" s="8">
+        <v>45233</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="128"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="40"/>
+      <c r="Q16" s="65"/>
+      <c r="R16" s="31"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="30"/>
+      <c r="U16" s="40"/>
+      <c r="V16" s="65"/>
+      <c r="W16" s="30"/>
+      <c r="X16" s="30"/>
+      <c r="Y16" s="30"/>
+      <c r="Z16" s="129"/>
+      <c r="AA16" s="59"/>
+    </row>
+    <row r="17" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="8">
+        <v>45234</v>
+      </c>
+      <c r="E17" s="8">
+        <v>45234</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="128"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="65"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="65"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="31"/>
+      <c r="T17" s="30"/>
+      <c r="U17" s="40"/>
+      <c r="V17" s="65"/>
+      <c r="W17" s="30"/>
+      <c r="X17" s="30"/>
+      <c r="Y17" s="30"/>
+      <c r="Z17" s="129"/>
+      <c r="AA17" s="59"/>
+    </row>
+    <row r="18" spans="2:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="17"/>
+      <c r="D18" s="8">
+        <v>45235</v>
+      </c>
+      <c r="E18" s="8">
+        <v>45235</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="130"/>
+      <c r="H18" s="131"/>
+      <c r="I18" s="131"/>
+      <c r="J18" s="131"/>
+      <c r="K18" s="132"/>
+      <c r="L18" s="133"/>
+      <c r="M18" s="131"/>
+      <c r="N18" s="131"/>
+      <c r="O18" s="131"/>
+      <c r="P18" s="132"/>
+      <c r="Q18" s="133"/>
+      <c r="R18" s="131"/>
+      <c r="S18" s="131"/>
+      <c r="T18" s="134"/>
+      <c r="U18" s="132"/>
+      <c r="V18" s="133"/>
+      <c r="W18" s="131"/>
+      <c r="X18" s="131"/>
+      <c r="Y18" s="131"/>
+      <c r="Z18" s="135"/>
+      <c r="AA18" s="59"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="V6:Z7"/>
+    <mergeCell ref="B3:E5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="G6:K7"/>
+    <mergeCell ref="L6:P7"/>
+    <mergeCell ref="Q6:U7"/>
+    <mergeCell ref="C7:E7"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" fitToHeight="0" orientation="landscape"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D5DC7C-4915-4BB3-B9DE-75E5E0D03399}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:AA17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.5703125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1"/>
+    </row>
+    <row r="2" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+    </row>
+    <row r="3" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="114" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="60"/>
+    </row>
+    <row r="4" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="114"/>
+      <c r="C4" s="114"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59"/>
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="59"/>
+      <c r="W4" s="59"/>
+      <c r="X4" s="59"/>
+      <c r="Y4" s="59"/>
+      <c r="Z4" s="59"/>
+      <c r="AA4" s="59"/>
+    </row>
+    <row r="5" spans="2:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="114"/>
+      <c r="C5" s="114"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="59"/>
+      <c r="R5" s="59"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="59"/>
+      <c r="V5" s="59"/>
+      <c r="W5" s="59"/>
+      <c r="X5" s="59"/>
+      <c r="Y5" s="59"/>
+      <c r="Z5" s="59"/>
+      <c r="AA5" s="59"/>
+    </row>
+    <row r="6" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="111" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="112" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="116">
+        <v>45236</v>
+      </c>
+      <c r="H6" s="117"/>
+      <c r="I6" s="117"/>
+      <c r="J6" s="117"/>
+      <c r="K6" s="117"/>
+      <c r="L6" s="118">
+        <v>45243</v>
+      </c>
+      <c r="M6" s="117"/>
+      <c r="N6" s="117"/>
+      <c r="O6" s="117"/>
+      <c r="P6" s="117"/>
+      <c r="Q6" s="118">
+        <v>45250</v>
+      </c>
+      <c r="R6" s="117"/>
+      <c r="S6" s="117"/>
+      <c r="T6" s="117"/>
+      <c r="U6" s="117"/>
+      <c r="V6" s="118">
+        <v>45257</v>
+      </c>
+      <c r="W6" s="117"/>
+      <c r="X6" s="117"/>
+      <c r="Y6" s="117"/>
+      <c r="Z6" s="119"/>
+      <c r="AA6" s="59"/>
+    </row>
+    <row r="7" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="111"/>
+      <c r="C7" s="113" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="120"/>
+      <c r="H7" s="108"/>
+      <c r="I7" s="108"/>
+      <c r="J7" s="108"/>
+      <c r="K7" s="108"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="108"/>
+      <c r="N7" s="108"/>
+      <c r="O7" s="108"/>
+      <c r="P7" s="108"/>
+      <c r="Q7" s="107"/>
+      <c r="R7" s="108"/>
+      <c r="S7" s="108"/>
+      <c r="T7" s="108"/>
+      <c r="U7" s="108"/>
+      <c r="V7" s="107"/>
+      <c r="W7" s="108"/>
+      <c r="X7" s="108"/>
+      <c r="Y7" s="108"/>
+      <c r="Z7" s="121"/>
+      <c r="AA7" s="59"/>
+    </row>
+    <row r="8" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="115" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="115"/>
+      <c r="D8" s="115" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="115" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="61"/>
+      <c r="G8" s="122">
+        <v>6</v>
+      </c>
+      <c r="H8" s="29">
+        <v>7</v>
+      </c>
+      <c r="I8" s="29">
+        <v>8</v>
+      </c>
+      <c r="J8" s="29">
+        <v>9</v>
+      </c>
+      <c r="K8" s="39">
+        <v>10</v>
+      </c>
+      <c r="L8" s="63">
+        <v>13</v>
+      </c>
+      <c r="M8" s="29">
+        <v>14</v>
+      </c>
+      <c r="N8" s="29">
+        <v>15</v>
+      </c>
+      <c r="O8" s="29">
+        <v>16</v>
+      </c>
+      <c r="P8" s="39">
+        <v>17</v>
+      </c>
+      <c r="Q8" s="63">
+        <v>20</v>
+      </c>
+      <c r="R8" s="29">
+        <v>21</v>
+      </c>
+      <c r="S8" s="29">
+        <v>22</v>
+      </c>
+      <c r="T8" s="29">
+        <v>23</v>
+      </c>
+      <c r="U8" s="39">
+        <v>24</v>
+      </c>
+      <c r="V8" s="63">
+        <v>27</v>
+      </c>
+      <c r="W8" s="29">
+        <v>28</v>
+      </c>
+      <c r="X8" s="29">
+        <v>29</v>
+      </c>
+      <c r="Y8" s="29">
+        <v>30</v>
+      </c>
+      <c r="Z8" s="123">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="59"/>
+    </row>
+    <row r="9" spans="2:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="115"/>
+      <c r="C9" s="115"/>
+      <c r="D9" s="115"/>
+      <c r="E9" s="115"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="124" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="P9" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="R9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="S9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="T9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="U9" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="V9" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="W9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="X9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z9" s="125" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA9" s="59"/>
+    </row>
+    <row r="10" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="126"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="84"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="83"/>
+      <c r="N10" s="83"/>
+      <c r="O10" s="83"/>
+      <c r="P10" s="84"/>
+      <c r="Q10" s="82"/>
+      <c r="R10" s="83"/>
+      <c r="S10" s="83"/>
+      <c r="T10" s="83"/>
+      <c r="U10" s="84"/>
+      <c r="V10" s="82"/>
+      <c r="W10" s="83"/>
+      <c r="X10" s="83"/>
+      <c r="Y10" s="83"/>
+      <c r="Z10" s="127"/>
+      <c r="AA10" s="59"/>
+    </row>
+    <row r="11" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="28">
+        <v>45236</v>
+      </c>
+      <c r="E11" s="28">
+        <v>45237</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="128"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="72"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="65"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="40"/>
+      <c r="V11" s="65"/>
+      <c r="W11" s="30"/>
+      <c r="X11" s="30"/>
+      <c r="Y11" s="30"/>
+      <c r="Z11" s="129"/>
+      <c r="AA11" s="59"/>
+    </row>
+    <row r="12" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="28">
+        <v>45238</v>
+      </c>
+      <c r="E12" s="28">
+        <v>45238</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="128"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="65"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="30"/>
+      <c r="U12" s="40"/>
+      <c r="V12" s="65"/>
+      <c r="W12" s="30"/>
+      <c r="X12" s="30"/>
+      <c r="Y12" s="30"/>
+      <c r="Z12" s="129"/>
+      <c r="AA12" s="59"/>
+    </row>
+    <row r="13" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="28">
+        <v>45239</v>
+      </c>
+      <c r="E13" s="28">
+        <v>45240</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="128"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="65"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="65"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30"/>
+      <c r="U13" s="40"/>
+      <c r="V13" s="65"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="30"/>
+      <c r="Y13" s="30"/>
+      <c r="Z13" s="129"/>
+      <c r="AA13" s="59"/>
+    </row>
+    <row r="14" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="28">
+        <v>45241</v>
+      </c>
+      <c r="E14" s="28">
+        <v>45243</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="128"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="73"/>
+      <c r="Q14" s="72"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
+      <c r="U14" s="40"/>
+      <c r="V14" s="65"/>
+      <c r="W14" s="30"/>
+      <c r="X14" s="30"/>
+      <c r="Y14" s="30"/>
+      <c r="Z14" s="129"/>
+      <c r="AA14" s="59"/>
+    </row>
+    <row r="15" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="28">
+        <v>45244</v>
+      </c>
+      <c r="E15" s="28">
+        <v>45245</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="128"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="65"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="32"/>
+      <c r="T15" s="32"/>
+      <c r="U15" s="40"/>
+      <c r="V15" s="65"/>
+      <c r="W15" s="30"/>
+      <c r="X15" s="30"/>
+      <c r="Y15" s="30"/>
+      <c r="Z15" s="129"/>
+      <c r="AA15" s="59"/>
+    </row>
+    <row r="16" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="28">
+        <v>45246</v>
+      </c>
+      <c r="E16" s="28">
+        <v>45247</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="128"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="40"/>
+      <c r="Q16" s="65"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="30"/>
+      <c r="U16" s="73"/>
+      <c r="V16" s="72"/>
+      <c r="W16" s="30"/>
+      <c r="X16" s="30"/>
+      <c r="Y16" s="30"/>
+      <c r="Z16" s="129"/>
+      <c r="AA16" s="59"/>
+    </row>
+    <row r="17" spans="2:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="28">
+        <v>45248</v>
+      </c>
+      <c r="E17" s="28">
+        <v>45248</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="130"/>
+      <c r="H17" s="131"/>
+      <c r="I17" s="131"/>
+      <c r="J17" s="131"/>
+      <c r="K17" s="132"/>
+      <c r="L17" s="133"/>
+      <c r="M17" s="131"/>
+      <c r="N17" s="131"/>
+      <c r="O17" s="131"/>
+      <c r="P17" s="132"/>
+      <c r="Q17" s="133"/>
+      <c r="R17" s="131"/>
+      <c r="S17" s="131"/>
+      <c r="T17" s="131"/>
+      <c r="U17" s="132"/>
+      <c r="V17" s="133"/>
+      <c r="W17" s="137"/>
+      <c r="X17" s="131"/>
+      <c r="Y17" s="131"/>
+      <c r="Z17" s="135"/>
+      <c r="AA17" s="59"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="L6:P7"/>
+    <mergeCell ref="Q6:U7"/>
+    <mergeCell ref="V6:Z7"/>
+    <mergeCell ref="B3:E5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="G6:K7"/>
+    <mergeCell ref="C7:E7"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" fitToHeight="0" orientation="landscape"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29FEE9A-2FAC-41D2-8C22-0B5777027BF1}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:AP19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.5703125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1"/>
+    </row>
+    <row r="2" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+    </row>
+    <row r="3" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="114" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="60"/>
+    </row>
+    <row r="4" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="114"/>
+      <c r="C4" s="114"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59"/>
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="59"/>
+      <c r="W4" s="59"/>
+      <c r="X4" s="59"/>
+      <c r="Y4" s="59"/>
+      <c r="Z4" s="59"/>
+      <c r="AA4" s="59"/>
+      <c r="AB4" s="59"/>
+      <c r="AC4" s="59"/>
+      <c r="AD4" s="59"/>
+      <c r="AE4" s="59"/>
+      <c r="AF4" s="59"/>
+      <c r="AG4" s="59"/>
+      <c r="AH4" s="59"/>
+      <c r="AI4" s="59"/>
+      <c r="AJ4" s="59"/>
+      <c r="AK4" s="59"/>
+      <c r="AL4" s="59"/>
+      <c r="AM4" s="59"/>
+      <c r="AN4" s="59"/>
+      <c r="AO4" s="59"/>
+      <c r="AP4" s="59"/>
+    </row>
+    <row r="5" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="114"/>
+      <c r="C5" s="114"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="59"/>
+      <c r="R5" s="59"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="59"/>
+      <c r="V5" s="59"/>
+      <c r="W5" s="59"/>
+      <c r="X5" s="59"/>
+      <c r="Y5" s="59"/>
+      <c r="Z5" s="59"/>
+      <c r="AA5" s="59"/>
+      <c r="AB5" s="59"/>
+      <c r="AC5" s="59"/>
+      <c r="AD5" s="59"/>
+      <c r="AE5" s="59"/>
+      <c r="AF5" s="59"/>
+      <c r="AG5" s="59"/>
+      <c r="AH5" s="59"/>
+      <c r="AI5" s="59"/>
+      <c r="AJ5" s="59"/>
+      <c r="AK5" s="59"/>
+      <c r="AL5" s="59"/>
+      <c r="AM5" s="59"/>
+      <c r="AN5" s="59"/>
+      <c r="AO5" s="59"/>
+      <c r="AP5" s="59"/>
+    </row>
+    <row r="6" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="111" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="112" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="116">
+        <v>45257</v>
+      </c>
+      <c r="H6" s="117"/>
+      <c r="I6" s="117"/>
+      <c r="J6" s="117"/>
+      <c r="K6" s="117"/>
+      <c r="L6" s="118">
+        <v>45264</v>
+      </c>
+      <c r="M6" s="117"/>
+      <c r="N6" s="117"/>
+      <c r="O6" s="117"/>
+      <c r="P6" s="117"/>
+      <c r="Q6" s="118">
+        <v>45271</v>
+      </c>
+      <c r="R6" s="117"/>
+      <c r="S6" s="117"/>
+      <c r="T6" s="117"/>
+      <c r="U6" s="117"/>
+      <c r="V6" s="118">
+        <v>45278</v>
+      </c>
+      <c r="W6" s="117"/>
+      <c r="X6" s="117"/>
+      <c r="Y6" s="117"/>
+      <c r="Z6" s="117"/>
+      <c r="AA6" s="118">
+        <v>45285</v>
+      </c>
+      <c r="AB6" s="117"/>
+      <c r="AC6" s="117"/>
+      <c r="AD6" s="117"/>
+      <c r="AE6" s="117"/>
+      <c r="AF6" s="118">
+        <v>45292</v>
+      </c>
+      <c r="AG6" s="117"/>
+      <c r="AH6" s="117"/>
+      <c r="AI6" s="117"/>
+      <c r="AJ6" s="117"/>
+      <c r="AK6" s="138">
+        <v>45299</v>
+      </c>
+      <c r="AL6" s="139"/>
+      <c r="AM6" s="139"/>
+      <c r="AN6" s="139"/>
+      <c r="AO6" s="140"/>
+      <c r="AP6" s="59"/>
+    </row>
+    <row r="7" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="111"/>
+      <c r="C7" s="113" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="120"/>
+      <c r="H7" s="108"/>
+      <c r="I7" s="108"/>
+      <c r="J7" s="108"/>
+      <c r="K7" s="108"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="108"/>
+      <c r="N7" s="108"/>
+      <c r="O7" s="108"/>
+      <c r="P7" s="108"/>
+      <c r="Q7" s="107"/>
+      <c r="R7" s="108"/>
+      <c r="S7" s="108"/>
+      <c r="T7" s="108"/>
+      <c r="U7" s="108"/>
+      <c r="V7" s="107"/>
+      <c r="W7" s="108"/>
+      <c r="X7" s="108"/>
+      <c r="Y7" s="108"/>
+      <c r="Z7" s="108"/>
+      <c r="AA7" s="107"/>
+      <c r="AB7" s="108"/>
+      <c r="AC7" s="108"/>
+      <c r="AD7" s="108"/>
+      <c r="AE7" s="108"/>
+      <c r="AF7" s="107"/>
+      <c r="AG7" s="108"/>
+      <c r="AH7" s="108"/>
+      <c r="AI7" s="108"/>
+      <c r="AJ7" s="108"/>
+      <c r="AK7" s="102"/>
+      <c r="AL7" s="103"/>
+      <c r="AM7" s="103"/>
+      <c r="AN7" s="103"/>
+      <c r="AO7" s="141"/>
+      <c r="AP7" s="59"/>
+    </row>
+    <row r="8" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="115" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="115"/>
+      <c r="D8" s="115" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="115" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="61"/>
+      <c r="G8" s="122">
+        <v>27</v>
+      </c>
+      <c r="H8" s="29">
+        <v>28</v>
+      </c>
+      <c r="I8" s="29">
+        <v>29</v>
+      </c>
+      <c r="J8" s="29">
+        <v>30</v>
+      </c>
+      <c r="K8" s="39">
+        <v>1</v>
+      </c>
+      <c r="L8" s="63">
+        <v>4</v>
+      </c>
+      <c r="M8" s="29">
+        <v>5</v>
+      </c>
+      <c r="N8" s="29">
+        <v>6</v>
+      </c>
+      <c r="O8" s="29">
+        <v>7</v>
+      </c>
+      <c r="P8" s="39">
+        <v>8</v>
+      </c>
+      <c r="Q8" s="63">
+        <v>11</v>
+      </c>
+      <c r="R8" s="29">
+        <v>12</v>
+      </c>
+      <c r="S8" s="29">
+        <v>13</v>
+      </c>
+      <c r="T8" s="29">
+        <v>14</v>
+      </c>
+      <c r="U8" s="39">
+        <v>15</v>
+      </c>
+      <c r="V8" s="63">
+        <v>18</v>
+      </c>
+      <c r="W8" s="29">
+        <v>19</v>
+      </c>
+      <c r="X8" s="29">
+        <v>20</v>
+      </c>
+      <c r="Y8" s="29">
+        <v>21</v>
+      </c>
+      <c r="Z8" s="39">
+        <v>22</v>
+      </c>
+      <c r="AA8" s="63">
+        <v>25</v>
+      </c>
+      <c r="AB8" s="29">
+        <v>26</v>
+      </c>
+      <c r="AC8" s="29">
+        <v>27</v>
+      </c>
+      <c r="AD8" s="29">
+        <v>28</v>
+      </c>
+      <c r="AE8" s="39">
+        <v>29</v>
+      </c>
+      <c r="AF8" s="63">
+        <v>1</v>
+      </c>
+      <c r="AG8" s="29">
+        <v>2</v>
+      </c>
+      <c r="AH8" s="29">
+        <v>3</v>
+      </c>
+      <c r="AI8" s="29">
+        <v>4</v>
+      </c>
+      <c r="AJ8" s="39">
+        <v>5</v>
+      </c>
+      <c r="AK8" s="63">
+        <v>8</v>
+      </c>
+      <c r="AL8" s="39">
+        <v>9</v>
+      </c>
+      <c r="AM8" s="29">
+        <v>10</v>
+      </c>
+      <c r="AN8" s="39">
+        <v>11</v>
+      </c>
+      <c r="AO8" s="123">
+        <v>12</v>
+      </c>
+      <c r="AP8" s="59"/>
+    </row>
+    <row r="9" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="115"/>
+      <c r="C9" s="115"/>
+      <c r="D9" s="115"/>
+      <c r="E9" s="115"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="124" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="P9" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="R9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="S9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="T9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="U9" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="V9" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="W9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="X9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z9" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA9" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE9" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF9" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ9" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK9" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="AM9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="AN9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO9" s="125" t="s">
+        <v>11</v>
+      </c>
+      <c r="AP9" s="59"/>
+    </row>
+    <row r="10" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="126"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="84"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="83"/>
+      <c r="N10" s="83"/>
+      <c r="O10" s="83"/>
+      <c r="P10" s="84"/>
+      <c r="Q10" s="82"/>
+      <c r="R10" s="83"/>
+      <c r="S10" s="83"/>
+      <c r="T10" s="83"/>
+      <c r="U10" s="84"/>
+      <c r="V10" s="82"/>
+      <c r="W10" s="83"/>
+      <c r="X10" s="83"/>
+      <c r="Y10" s="83"/>
+      <c r="Z10" s="84"/>
+      <c r="AA10" s="82"/>
+      <c r="AB10" s="83"/>
+      <c r="AC10" s="83"/>
+      <c r="AD10" s="83"/>
+      <c r="AE10" s="84"/>
+      <c r="AF10" s="82"/>
+      <c r="AG10" s="83"/>
+      <c r="AH10" s="83"/>
+      <c r="AI10" s="83"/>
+      <c r="AJ10" s="84"/>
+      <c r="AK10" s="82"/>
+      <c r="AL10" s="83"/>
+      <c r="AM10" s="83"/>
+      <c r="AN10" s="83"/>
+      <c r="AO10" s="127"/>
+      <c r="AP10" s="59"/>
+    </row>
+    <row r="11" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="36">
+        <v>45249</v>
+      </c>
+      <c r="E11" s="36">
+        <v>45253</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="128"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="74"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="65"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="40"/>
+      <c r="V11" s="65"/>
+      <c r="W11" s="30"/>
+      <c r="X11" s="30"/>
+      <c r="Y11" s="30"/>
+      <c r="Z11" s="40"/>
+      <c r="AA11" s="65"/>
+      <c r="AB11" s="30"/>
+      <c r="AC11" s="30"/>
+      <c r="AD11" s="30"/>
+      <c r="AE11" s="40"/>
+      <c r="AF11" s="65"/>
+      <c r="AG11" s="30"/>
+      <c r="AH11" s="30"/>
+      <c r="AI11" s="30"/>
+      <c r="AJ11" s="40"/>
+      <c r="AK11" s="65"/>
+      <c r="AL11" s="30"/>
+      <c r="AM11" s="30"/>
+      <c r="AN11" s="30"/>
+      <c r="AO11" s="129"/>
+      <c r="AP11" s="59"/>
+    </row>
+    <row r="12" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="36">
+        <v>45254</v>
+      </c>
+      <c r="E12" s="36">
+        <v>45256</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="128"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="65"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="30"/>
+      <c r="U12" s="40"/>
+      <c r="V12" s="65"/>
+      <c r="W12" s="30"/>
+      <c r="X12" s="30"/>
+      <c r="Y12" s="30"/>
+      <c r="Z12" s="40"/>
+      <c r="AA12" s="65"/>
+      <c r="AB12" s="30"/>
+      <c r="AC12" s="30"/>
+      <c r="AD12" s="30"/>
+      <c r="AE12" s="40"/>
+      <c r="AF12" s="65"/>
+      <c r="AG12" s="30"/>
+      <c r="AH12" s="30"/>
+      <c r="AI12" s="30"/>
+      <c r="AJ12" s="40"/>
+      <c r="AK12" s="65"/>
+      <c r="AL12" s="30"/>
+      <c r="AM12" s="30"/>
+      <c r="AN12" s="30"/>
+      <c r="AO12" s="129"/>
+      <c r="AP12" s="59"/>
+    </row>
+    <row r="13" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="36">
+        <v>45257</v>
+      </c>
+      <c r="E13" s="36">
+        <v>45258</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="128"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="65"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="74"/>
+      <c r="R13" s="33"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30"/>
+      <c r="U13" s="40"/>
+      <c r="V13" s="65"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="30"/>
+      <c r="Y13" s="30"/>
+      <c r="Z13" s="40"/>
+      <c r="AA13" s="65"/>
+      <c r="AB13" s="30"/>
+      <c r="AC13" s="30"/>
+      <c r="AD13" s="30"/>
+      <c r="AE13" s="40"/>
+      <c r="AF13" s="65"/>
+      <c r="AG13" s="30"/>
+      <c r="AH13" s="30"/>
+      <c r="AI13" s="30"/>
+      <c r="AJ13" s="40"/>
+      <c r="AK13" s="65"/>
+      <c r="AL13" s="30"/>
+      <c r="AM13" s="30"/>
+      <c r="AN13" s="30"/>
+      <c r="AO13" s="129"/>
+      <c r="AP13" s="59"/>
+    </row>
+    <row r="14" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="36">
+        <v>45259</v>
+      </c>
+      <c r="E14" s="36">
+        <v>45262</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="128"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="65"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="33"/>
+      <c r="T14" s="33"/>
+      <c r="U14" s="41"/>
+      <c r="V14" s="74"/>
+      <c r="W14" s="30"/>
+      <c r="X14" s="30"/>
+      <c r="Y14" s="30"/>
+      <c r="Z14" s="40"/>
+      <c r="AA14" s="65"/>
+      <c r="AB14" s="30"/>
+      <c r="AC14" s="30"/>
+      <c r="AD14" s="30"/>
+      <c r="AE14" s="40"/>
+      <c r="AF14" s="65"/>
+      <c r="AG14" s="30"/>
+      <c r="AH14" s="30"/>
+      <c r="AI14" s="30"/>
+      <c r="AJ14" s="40"/>
+      <c r="AK14" s="65"/>
+      <c r="AL14" s="30"/>
+      <c r="AM14" s="30"/>
+      <c r="AN14" s="30"/>
+      <c r="AO14" s="129"/>
+      <c r="AP14" s="59"/>
+    </row>
+    <row r="15" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="36">
+        <v>45263</v>
+      </c>
+      <c r="E15" s="36">
+        <v>45266</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="128"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="65"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="30"/>
+      <c r="U15" s="40"/>
+      <c r="V15" s="65"/>
+      <c r="W15" s="33"/>
+      <c r="X15" s="33"/>
+      <c r="Y15" s="33"/>
+      <c r="Z15" s="41"/>
+      <c r="AA15" s="65"/>
+      <c r="AB15" s="30"/>
+      <c r="AC15" s="30"/>
+      <c r="AD15" s="30"/>
+      <c r="AE15" s="40"/>
+      <c r="AF15" s="65"/>
+      <c r="AG15" s="30"/>
+      <c r="AH15" s="30"/>
+      <c r="AI15" s="30"/>
+      <c r="AJ15" s="40"/>
+      <c r="AK15" s="65"/>
+      <c r="AL15" s="30"/>
+      <c r="AM15" s="30"/>
+      <c r="AN15" s="30"/>
+      <c r="AO15" s="129"/>
+      <c r="AP15" s="59"/>
+    </row>
+    <row r="16" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="36">
+        <v>45267</v>
+      </c>
+      <c r="E16" s="36">
+        <v>45269</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="128"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="40"/>
+      <c r="Q16" s="65"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="30"/>
+      <c r="U16" s="40"/>
+      <c r="V16" s="65"/>
+      <c r="W16" s="30"/>
+      <c r="X16" s="30"/>
+      <c r="Y16" s="30"/>
+      <c r="Z16" s="40"/>
+      <c r="AA16" s="74"/>
+      <c r="AB16" s="33"/>
+      <c r="AC16" s="33"/>
+      <c r="AD16" s="30"/>
+      <c r="AE16" s="40"/>
+      <c r="AF16" s="65"/>
+      <c r="AG16" s="30"/>
+      <c r="AH16" s="30"/>
+      <c r="AI16" s="30"/>
+      <c r="AJ16" s="40"/>
+      <c r="AK16" s="65"/>
+      <c r="AL16" s="30"/>
+      <c r="AM16" s="30"/>
+      <c r="AN16" s="30"/>
+      <c r="AO16" s="129"/>
+      <c r="AP16" s="59"/>
+    </row>
+    <row r="17" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="36">
+        <v>45270</v>
+      </c>
+      <c r="E17" s="36">
+        <v>45274</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="128"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="65"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="65"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="30"/>
+      <c r="T17" s="30"/>
+      <c r="U17" s="40"/>
+      <c r="V17" s="65"/>
+      <c r="W17" s="30"/>
+      <c r="X17" s="30"/>
+      <c r="Y17" s="30"/>
+      <c r="Z17" s="40"/>
+      <c r="AA17" s="65"/>
+      <c r="AB17" s="30"/>
+      <c r="AC17" s="30"/>
+      <c r="AD17" s="33"/>
+      <c r="AE17" s="41"/>
+      <c r="AF17" s="74"/>
+      <c r="AG17" s="33"/>
+      <c r="AH17" s="33"/>
+      <c r="AI17" s="30"/>
+      <c r="AJ17" s="40"/>
+      <c r="AK17" s="65"/>
+      <c r="AL17" s="30"/>
+      <c r="AM17" s="30"/>
+      <c r="AN17" s="30"/>
+      <c r="AO17" s="129"/>
+      <c r="AP17" s="59"/>
+    </row>
+    <row r="18" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="36">
+        <v>45275</v>
+      </c>
+      <c r="E18" s="36">
+        <v>45277</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="128"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="65"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="30"/>
+      <c r="U18" s="40"/>
+      <c r="V18" s="65"/>
+      <c r="W18" s="30"/>
+      <c r="X18" s="30"/>
+      <c r="Y18" s="30"/>
+      <c r="Z18" s="40"/>
+      <c r="AA18" s="65"/>
+      <c r="AB18" s="30"/>
+      <c r="AC18" s="30"/>
+      <c r="AD18" s="30"/>
+      <c r="AE18" s="40"/>
+      <c r="AF18" s="65"/>
+      <c r="AG18" s="30"/>
+      <c r="AH18" s="30"/>
+      <c r="AI18" s="33"/>
+      <c r="AJ18" s="41"/>
+      <c r="AK18" s="74"/>
+      <c r="AL18" s="30"/>
+      <c r="AM18" s="30"/>
+      <c r="AN18" s="30"/>
+      <c r="AO18" s="129"/>
+      <c r="AP18" s="59"/>
+    </row>
+    <row r="19" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="36">
+        <v>45278</v>
+      </c>
+      <c r="E19" s="36">
+        <v>45279</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="130"/>
+      <c r="H19" s="131"/>
+      <c r="I19" s="131"/>
+      <c r="J19" s="131"/>
+      <c r="K19" s="132"/>
+      <c r="L19" s="133"/>
+      <c r="M19" s="131"/>
+      <c r="N19" s="131"/>
+      <c r="O19" s="131"/>
+      <c r="P19" s="132"/>
+      <c r="Q19" s="133"/>
+      <c r="R19" s="131"/>
+      <c r="S19" s="131"/>
+      <c r="T19" s="131"/>
+      <c r="U19" s="132"/>
+      <c r="V19" s="133"/>
+      <c r="W19" s="131"/>
+      <c r="X19" s="131"/>
+      <c r="Y19" s="131"/>
+      <c r="Z19" s="132"/>
+      <c r="AA19" s="133"/>
+      <c r="AB19" s="131"/>
+      <c r="AC19" s="131"/>
+      <c r="AD19" s="131"/>
+      <c r="AE19" s="132"/>
+      <c r="AF19" s="133"/>
+      <c r="AG19" s="131"/>
+      <c r="AH19" s="131"/>
+      <c r="AI19" s="131"/>
+      <c r="AJ19" s="132"/>
+      <c r="AK19" s="133"/>
+      <c r="AL19" s="142"/>
+      <c r="AM19" s="142"/>
+      <c r="AN19" s="131"/>
+      <c r="AO19" s="135"/>
+      <c r="AP19" s="59"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="AA6:AE7"/>
+    <mergeCell ref="AF6:AJ7"/>
+    <mergeCell ref="AK6:AO7"/>
+    <mergeCell ref="G6:K7"/>
+    <mergeCell ref="L6:P7"/>
+    <mergeCell ref="Q6:U7"/>
+    <mergeCell ref="V6:Z7"/>
+    <mergeCell ref="B3:E5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" fitToHeight="0" orientation="landscape"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF07BA14-4B82-42BF-886F-9D48DA31A689}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:AA15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:AA15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.5703125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1"/>
+    </row>
+    <row r="2" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+    </row>
+    <row r="3" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="114" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="60"/>
+    </row>
+    <row r="4" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="114"/>
+      <c r="C4" s="114"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59"/>
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="59"/>
+      <c r="W4" s="59"/>
+      <c r="X4" s="59"/>
+      <c r="Y4" s="59"/>
+      <c r="Z4" s="59"/>
+      <c r="AA4" s="59"/>
+    </row>
+    <row r="5" spans="2:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="114"/>
+      <c r="C5" s="114"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="59"/>
+      <c r="R5" s="59"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="59"/>
+      <c r="V5" s="59"/>
+      <c r="W5" s="59"/>
+      <c r="X5" s="59"/>
+      <c r="Y5" s="59"/>
+      <c r="Z5" s="59"/>
+      <c r="AA5" s="59"/>
+    </row>
+    <row r="6" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="111" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="112" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="143">
+        <v>45299</v>
+      </c>
+      <c r="H6" s="139"/>
+      <c r="I6" s="139"/>
+      <c r="J6" s="139"/>
+      <c r="K6" s="144"/>
+      <c r="L6" s="118">
+        <v>45306</v>
+      </c>
+      <c r="M6" s="117"/>
+      <c r="N6" s="117"/>
+      <c r="O6" s="117"/>
+      <c r="P6" s="117"/>
+      <c r="Q6" s="138">
+        <v>45313</v>
+      </c>
+      <c r="R6" s="139"/>
+      <c r="S6" s="139"/>
+      <c r="T6" s="139"/>
+      <c r="U6" s="144"/>
+      <c r="V6" s="138">
+        <v>45320</v>
+      </c>
+      <c r="W6" s="139"/>
+      <c r="X6" s="139"/>
+      <c r="Y6" s="139"/>
+      <c r="Z6" s="140"/>
+      <c r="AA6" s="59"/>
+    </row>
+    <row r="7" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="111"/>
+      <c r="C7" s="113" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="145"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="103"/>
+      <c r="J7" s="103"/>
+      <c r="K7" s="104"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="108"/>
+      <c r="N7" s="108"/>
+      <c r="O7" s="108"/>
+      <c r="P7" s="108"/>
+      <c r="Q7" s="102"/>
+      <c r="R7" s="103"/>
+      <c r="S7" s="103"/>
+      <c r="T7" s="103"/>
+      <c r="U7" s="104"/>
+      <c r="V7" s="102"/>
+      <c r="W7" s="103"/>
+      <c r="X7" s="103"/>
+      <c r="Y7" s="103"/>
+      <c r="Z7" s="141"/>
+      <c r="AA7" s="59"/>
+    </row>
+    <row r="8" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="115" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="115"/>
+      <c r="D8" s="115" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="115" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="61"/>
+      <c r="G8" s="122">
+        <v>8</v>
+      </c>
+      <c r="H8" s="39">
+        <v>9</v>
+      </c>
+      <c r="I8" s="29">
+        <v>10</v>
+      </c>
+      <c r="J8" s="39">
+        <v>11</v>
+      </c>
+      <c r="K8" s="39">
+        <v>12</v>
+      </c>
+      <c r="L8" s="75">
+        <v>15</v>
+      </c>
+      <c r="M8" s="29">
+        <v>16</v>
+      </c>
+      <c r="N8" s="39">
+        <v>17</v>
+      </c>
+      <c r="O8" s="29">
+        <v>18</v>
+      </c>
+      <c r="P8" s="39">
+        <v>19</v>
+      </c>
+      <c r="Q8" s="63">
+        <v>22</v>
+      </c>
+      <c r="R8" s="39">
+        <v>23</v>
+      </c>
+      <c r="S8" s="29">
+        <v>24</v>
+      </c>
+      <c r="T8" s="39">
+        <v>25</v>
+      </c>
+      <c r="U8" s="39">
+        <v>26</v>
+      </c>
+      <c r="V8" s="63">
+        <v>29</v>
+      </c>
+      <c r="W8" s="29">
+        <v>30</v>
+      </c>
+      <c r="X8" s="29">
+        <v>31</v>
+      </c>
+      <c r="Y8" s="29">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="123">
+        <v>2</v>
+      </c>
+      <c r="AA8" s="59"/>
+    </row>
+    <row r="9" spans="2:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="115"/>
+      <c r="C9" s="115"/>
+      <c r="D9" s="115"/>
+      <c r="E9" s="115"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="124" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="P9" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="R9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="S9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="T9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="U9" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="V9" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="W9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="X9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z9" s="125" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA9" s="59"/>
+    </row>
+    <row r="10" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="126"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="84"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="83"/>
+      <c r="N10" s="83"/>
+      <c r="O10" s="83"/>
+      <c r="P10" s="84"/>
+      <c r="Q10" s="82"/>
+      <c r="R10" s="83"/>
+      <c r="S10" s="83"/>
+      <c r="T10" s="83"/>
+      <c r="U10" s="84"/>
+      <c r="V10" s="82"/>
+      <c r="W10" s="83"/>
+      <c r="X10" s="83"/>
+      <c r="Y10" s="83"/>
+      <c r="Z10" s="127"/>
+      <c r="AA10" s="59"/>
+    </row>
+    <row r="11" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="37">
+        <v>45280</v>
+      </c>
+      <c r="E11" s="37">
+        <v>45281</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="128"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="77"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="65"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="40"/>
+      <c r="V11" s="65"/>
+      <c r="W11" s="30"/>
+      <c r="X11" s="30"/>
+      <c r="Y11" s="30"/>
+      <c r="Z11" s="129"/>
+      <c r="AA11" s="59"/>
+    </row>
+    <row r="12" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="37">
+        <v>45282</v>
+      </c>
+      <c r="E12" s="37">
+        <v>45282</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="128"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="76"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="65"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="30"/>
+      <c r="U12" s="40"/>
+      <c r="V12" s="65"/>
+      <c r="W12" s="30"/>
+      <c r="X12" s="30"/>
+      <c r="Y12" s="30"/>
+      <c r="Z12" s="129"/>
+      <c r="AA12" s="59"/>
+    </row>
+    <row r="13" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="37">
+        <v>45283</v>
+      </c>
+      <c r="E13" s="37">
+        <v>45283</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="128"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="65"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="65"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30"/>
+      <c r="U13" s="40"/>
+      <c r="V13" s="65"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="30"/>
+      <c r="Y13" s="30"/>
+      <c r="Z13" s="129"/>
+      <c r="AA13" s="59"/>
+    </row>
+    <row r="14" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="37">
+        <v>45284</v>
+      </c>
+      <c r="E14" s="37">
+        <v>45285</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="128"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="65"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
+      <c r="U14" s="40"/>
+      <c r="V14" s="65"/>
+      <c r="W14" s="30"/>
+      <c r="X14" s="30"/>
+      <c r="Y14" s="30"/>
+      <c r="Z14" s="129"/>
+      <c r="AA14" s="59"/>
+    </row>
+    <row r="15" spans="2:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="37">
+        <v>45286</v>
+      </c>
+      <c r="E15" s="37">
+        <v>45287</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="130"/>
+      <c r="H15" s="131"/>
+      <c r="I15" s="131"/>
+      <c r="J15" s="131"/>
+      <c r="K15" s="132"/>
+      <c r="L15" s="133"/>
+      <c r="M15" s="131"/>
+      <c r="N15" s="131"/>
+      <c r="O15" s="131"/>
+      <c r="P15" s="146"/>
+      <c r="Q15" s="147"/>
+      <c r="R15" s="131"/>
+      <c r="S15" s="131"/>
+      <c r="T15" s="131"/>
+      <c r="U15" s="132"/>
+      <c r="V15" s="133"/>
+      <c r="W15" s="131"/>
+      <c r="X15" s="131"/>
+      <c r="Y15" s="131"/>
+      <c r="Z15" s="135"/>
+      <c r="AA15" s="59"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="G6:K7"/>
+    <mergeCell ref="L6:P7"/>
+    <mergeCell ref="Q6:U7"/>
+    <mergeCell ref="V6:Z7"/>
+    <mergeCell ref="B3:E5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" fitToHeight="0" orientation="landscape"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83820A67-1D0D-4613-BBD6-229CA836852A}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:AA17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AF14" sqref="AF14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.5703125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1"/>
+    </row>
+    <row r="2" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+    </row>
+    <row r="3" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="114" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="60"/>
+    </row>
+    <row r="4" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="114"/>
+      <c r="C4" s="114"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59"/>
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="59"/>
+      <c r="W4" s="59"/>
+      <c r="X4" s="59"/>
+      <c r="Y4" s="59"/>
+      <c r="Z4" s="59"/>
+      <c r="AA4" s="59"/>
+    </row>
+    <row r="5" spans="2:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="114"/>
+      <c r="C5" s="114"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="59"/>
+      <c r="R5" s="59"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="59"/>
+      <c r="V5" s="59"/>
+      <c r="W5" s="59"/>
+      <c r="X5" s="59"/>
+      <c r="Y5" s="59"/>
+      <c r="Z5" s="59"/>
+      <c r="AA5" s="59"/>
+    </row>
+    <row r="6" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="111" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="112" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="99">
+        <v>45299</v>
+      </c>
+      <c r="H6" s="100"/>
+      <c r="I6" s="100"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="101"/>
+      <c r="L6" s="105">
+        <v>45306</v>
+      </c>
+      <c r="M6" s="106"/>
+      <c r="N6" s="106"/>
+      <c r="O6" s="106"/>
+      <c r="P6" s="106"/>
+      <c r="Q6" s="99">
+        <v>45313</v>
+      </c>
+      <c r="R6" s="100"/>
+      <c r="S6" s="100"/>
+      <c r="T6" s="100"/>
+      <c r="U6" s="101"/>
+      <c r="V6" s="99">
+        <v>45320</v>
+      </c>
+      <c r="W6" s="100"/>
+      <c r="X6" s="100"/>
+      <c r="Y6" s="100"/>
+      <c r="Z6" s="109"/>
+      <c r="AA6" s="59"/>
+    </row>
+    <row r="7" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="111"/>
+      <c r="C7" s="113" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="103"/>
+      <c r="J7" s="103"/>
+      <c r="K7" s="104"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="108"/>
+      <c r="N7" s="108"/>
+      <c r="O7" s="108"/>
+      <c r="P7" s="108"/>
+      <c r="Q7" s="102"/>
+      <c r="R7" s="103"/>
+      <c r="S7" s="103"/>
+      <c r="T7" s="103"/>
+      <c r="U7" s="104"/>
+      <c r="V7" s="102"/>
+      <c r="W7" s="103"/>
+      <c r="X7" s="103"/>
+      <c r="Y7" s="103"/>
+      <c r="Z7" s="110"/>
+      <c r="AA7" s="59"/>
+    </row>
+    <row r="8" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="115" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="115"/>
+      <c r="D8" s="115" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="115" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="61"/>
+      <c r="G8" s="63">
+        <v>8</v>
+      </c>
+      <c r="H8" s="39">
+        <v>9</v>
+      </c>
+      <c r="I8" s="29">
+        <v>10</v>
+      </c>
+      <c r="J8" s="39">
+        <v>11</v>
+      </c>
+      <c r="K8" s="39">
+        <v>12</v>
+      </c>
+      <c r="L8" s="75">
+        <v>15</v>
+      </c>
+      <c r="M8" s="29">
+        <v>16</v>
+      </c>
+      <c r="N8" s="39">
+        <v>17</v>
+      </c>
+      <c r="O8" s="29">
+        <v>18</v>
+      </c>
+      <c r="P8" s="39">
+        <v>19</v>
+      </c>
+      <c r="Q8" s="63">
+        <v>22</v>
+      </c>
+      <c r="R8" s="39">
+        <v>23</v>
+      </c>
+      <c r="S8" s="29">
+        <v>24</v>
+      </c>
+      <c r="T8" s="39">
+        <v>25</v>
+      </c>
+      <c r="U8" s="39">
+        <v>26</v>
+      </c>
+      <c r="V8" s="63">
+        <v>29</v>
+      </c>
+      <c r="W8" s="29">
+        <v>30</v>
+      </c>
+      <c r="X8" s="29">
+        <v>31</v>
+      </c>
+      <c r="Y8" s="29">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="64">
+        <v>2</v>
+      </c>
+      <c r="AA8" s="59"/>
+    </row>
+    <row r="9" spans="2:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="115"/>
+      <c r="C9" s="115"/>
+      <c r="D9" s="115"/>
+      <c r="E9" s="115"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="P9" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="R9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="S9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="T9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="U9" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="V9" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="W9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="X9" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y9" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z9" s="89" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA9" s="59"/>
+    </row>
+    <row r="10" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="84"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="83"/>
+      <c r="N10" s="83"/>
+      <c r="O10" s="83"/>
+      <c r="P10" s="84"/>
+      <c r="Q10" s="82"/>
+      <c r="R10" s="83"/>
+      <c r="S10" s="83"/>
+      <c r="T10" s="83"/>
+      <c r="U10" s="84"/>
+      <c r="V10" s="82"/>
+      <c r="W10" s="83"/>
+      <c r="X10" s="83"/>
+      <c r="Y10" s="83"/>
+      <c r="Z10" s="85"/>
+      <c r="AA10" s="59"/>
+    </row>
+    <row r="11" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="38">
+        <v>45288</v>
+      </c>
+      <c r="E11" s="38">
+        <v>45289</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="65"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="35"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="40"/>
+      <c r="V11" s="65"/>
+      <c r="W11" s="30"/>
+      <c r="X11" s="30"/>
+      <c r="Y11" s="30"/>
+      <c r="Z11" s="66"/>
+      <c r="AA11" s="59"/>
+    </row>
+    <row r="12" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="38">
+        <v>45290</v>
+      </c>
+      <c r="E12" s="38">
+        <v>45291</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="65"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="35"/>
+      <c r="U12" s="42"/>
+      <c r="V12" s="65"/>
+      <c r="W12" s="30"/>
+      <c r="X12" s="30"/>
+      <c r="Y12" s="30"/>
+      <c r="Z12" s="66"/>
+      <c r="AA12" s="59"/>
+    </row>
+    <row r="13" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="38">
+        <v>45292</v>
+      </c>
+      <c r="E13" s="38">
+        <v>45292</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="65"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="65"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30"/>
+      <c r="U13" s="40"/>
+      <c r="V13" s="80"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="30"/>
+      <c r="Y13" s="30"/>
+      <c r="Z13" s="66"/>
+      <c r="AA13" s="59"/>
+    </row>
+    <row r="14" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="38">
+        <v>45293</v>
+      </c>
+      <c r="E14" s="38">
+        <v>45293</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="65"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
+      <c r="U14" s="40"/>
+      <c r="V14" s="65"/>
+      <c r="W14" s="35"/>
+      <c r="X14" s="30"/>
+      <c r="Y14" s="30"/>
+      <c r="Z14" s="66"/>
+      <c r="AA14" s="59"/>
+    </row>
+    <row r="15" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="38">
+        <v>45294</v>
+      </c>
+      <c r="E15" s="38">
+        <v>45294</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="65"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="30"/>
+      <c r="U15" s="40"/>
+      <c r="V15" s="65"/>
+      <c r="W15" s="30"/>
+      <c r="X15" s="35"/>
+      <c r="Y15" s="30"/>
+      <c r="Z15" s="66"/>
+      <c r="AA15" s="59"/>
+    </row>
+    <row r="16" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="38">
+        <v>45296</v>
+      </c>
+      <c r="E16" s="38">
+        <v>45296</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="40"/>
+      <c r="Q16" s="65"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="30"/>
+      <c r="U16" s="40"/>
+      <c r="V16" s="65"/>
+      <c r="W16" s="30"/>
+      <c r="X16" s="30"/>
+      <c r="Y16" s="35"/>
+      <c r="Z16" s="66"/>
+      <c r="AA16" s="59"/>
+    </row>
+    <row r="17" spans="2:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="38">
+        <v>45296</v>
+      </c>
+      <c r="E17" s="38">
+        <v>45296</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="68"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="68"/>
+      <c r="N17" s="68"/>
+      <c r="O17" s="68"/>
+      <c r="P17" s="71"/>
+      <c r="Q17" s="67"/>
+      <c r="R17" s="68"/>
+      <c r="S17" s="68"/>
+      <c r="T17" s="68"/>
+      <c r="U17" s="71"/>
+      <c r="V17" s="67"/>
+      <c r="W17" s="68"/>
+      <c r="X17" s="68"/>
+      <c r="Y17" s="68"/>
+      <c r="Z17" s="81"/>
+      <c r="AA17" s="59"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="G6:K7"/>
+    <mergeCell ref="L6:P7"/>
+    <mergeCell ref="Q6:U7"/>
+    <mergeCell ref="V6:Z7"/>
+    <mergeCell ref="B3:E5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" fitToHeight="0" orientation="landscape"/>
+</worksheet>
 </file>
</xml_diff>